<commit_message>
Add new participant data files and update AHP analysis to dynamically load Excel files; remove obsolete files
</commit_message>
<xml_diff>
--- a/AHP/ahp1.xlsx
+++ b/AHP/ahp1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaime\Desktop\TUD\DSE\Ekranoplan-DSE\AHP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9906906-F715-476E-8AEB-F4F9B36B1CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38058DD-F5BB-49ED-B34A-42340AF9BCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94C62CCA-CA46-4362-8D9B-A7BDF927CB06}"/>
   </bookViews>
@@ -41,41 +41,41 @@
     <t>AHP data</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>wrt C1</t>
-  </si>
-  <si>
-    <t>wrt C2</t>
-  </si>
-  <si>
-    <t>wrt C3</t>
-  </si>
-  <si>
-    <t>wrt C4</t>
-  </si>
-  <si>
-    <t>wrt C5</t>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Sustainability</t>
+  </si>
+  <si>
+    <t>Time to complete mission</t>
+  </si>
+  <si>
+    <t>Rough Sea Tolerance</t>
+  </si>
+  <si>
+    <t>Design Complexity</t>
+  </si>
+  <si>
+    <t>wrt Cost</t>
+  </si>
+  <si>
+    <t>wrt Sustainability</t>
+  </si>
+  <si>
+    <t>wrt Time</t>
+  </si>
+  <si>
+    <t>wrt Rough Sea</t>
+  </si>
+  <si>
+    <t>wrt Complexity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,10 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,20 +465,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3B51A8-C0DB-4B9E-8DE5-C441BE79AABF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -484,8 +501,9 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,19 +511,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E3" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -514,16 +533,17 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -533,13 +553,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -552,8 +573,9 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -564,6 +586,30 @@
       <c r="G7" s="2">
         <v>1</v>
       </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I11" s="4"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="4"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I13" s="4"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="4"/>
+      <c r="J14" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -767,20 +813,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="21c71b5b-54a6-4753-8f4b-20b8bb49b2a6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="21c71b5b-54a6-4753-8f4b-20b8bb49b2a6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,14 +849,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F45A72CE-FF17-4851-872B-3BDF847EA5BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CA09D2-6585-41AA-B5DA-DEE7EAECA1CF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -825,4 +863,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F45A72CE-FF17-4851-872B-3BDF847EA5BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>